<commit_message>
double trouble and round  2
</commit_message>
<xml_diff>
--- a/2020AAnswers.xlsx
+++ b/2020AAnswers.xlsx
@@ -711,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K15" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="O31" sqref="O31"/>
+    <sheetView tabSelected="1" topLeftCell="B8" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -782,8 +782,8 @@
       <c r="E2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="2" t="s">
-        <v>78</v>
+      <c r="O2" s="10" t="s">
+        <v>45</v>
       </c>
       <c r="P2" s="10" t="s">
         <v>45</v>
@@ -799,8 +799,8 @@
       <c r="D3" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>78</v>
+      <c r="F3" s="10" t="s">
+        <v>15</v>
       </c>
       <c r="N3" s="3" t="s">
         <v>78</v>
@@ -822,8 +822,8 @@
       <c r="E4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="O4" s="2" t="s">
-        <v>78</v>
+      <c r="O4" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="P4" s="10" t="s">
         <v>47</v>
@@ -862,8 +862,8 @@
       <c r="E6" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="O6" s="2" t="s">
-        <v>78</v>
+      <c r="O6" s="10" t="s">
+        <v>50</v>
       </c>
       <c r="P6" s="10" t="s">
         <v>49</v>
@@ -879,8 +879,8 @@
       <c r="D7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>78</v>
+      <c r="F7" s="13" t="s">
+        <v>19</v>
       </c>
       <c r="N7" s="3" t="s">
         <v>78</v>
@@ -902,8 +902,8 @@
       <c r="E8" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="O8" s="2" t="s">
-        <v>78</v>
+      <c r="O8" s="10" t="s">
+        <v>51</v>
       </c>
       <c r="P8" s="10" t="s">
         <v>51</v>
@@ -942,8 +942,8 @@
       <c r="E10" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="O10" s="2" t="s">
-        <v>78</v>
+      <c r="O10" s="10" t="s">
+        <v>53</v>
       </c>
       <c r="P10" s="10" t="s">
         <v>53</v>
@@ -959,8 +959,8 @@
       <c r="D11" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>78</v>
+      <c r="F11" s="10" t="s">
+        <v>24</v>
       </c>
       <c r="N11" s="3" t="s">
         <v>78</v>
@@ -972,7 +972,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="2:17" ht="19" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:17" ht="38" x14ac:dyDescent="0.2">
       <c r="C12">
         <v>3</v>
       </c>
@@ -982,8 +982,8 @@
       <c r="E12" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="O12" s="2" t="s">
-        <v>78</v>
+      <c r="O12" s="10" t="s">
+        <v>55</v>
       </c>
       <c r="P12" s="10" t="s">
         <v>55</v>
@@ -1022,8 +1022,8 @@
       <c r="E14" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="O14" s="2" t="s">
-        <v>78</v>
+      <c r="O14" s="10" t="s">
+        <v>57</v>
       </c>
       <c r="P14" s="10" t="s">
         <v>57</v>
@@ -1039,8 +1039,8 @@
       <c r="D15" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>78</v>
+      <c r="F15" s="10" t="s">
+        <v>28</v>
       </c>
       <c r="N15" s="3" t="s">
         <v>78</v>
@@ -1062,8 +1062,8 @@
       <c r="E16" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="O16" s="2" t="s">
-        <v>78</v>
+      <c r="O16" s="10" t="s">
+        <v>59</v>
       </c>
       <c r="P16" s="10" t="s">
         <v>59</v>
@@ -1141,8 +1141,8 @@
         <f>B20</f>
         <v>Pygmy Spotted Skunk</v>
       </c>
-      <c r="F20" s="3" t="s">
-        <v>78</v>
+      <c r="F20" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="N20" s="3" t="s">
         <v>78</v>
@@ -1222,8 +1222,8 @@
       <c r="D24" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F24" s="3" t="s">
-        <v>78</v>
+      <c r="F24" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="N24" s="3" t="s">
         <v>78</v>
@@ -1302,8 +1302,8 @@
       <c r="D28" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F28" s="3" t="s">
-        <v>78</v>
+      <c r="F28" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="N28" s="3" t="s">
         <v>78</v>
@@ -1382,8 +1382,8 @@
       <c r="D32" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="F32" s="3" t="s">
-        <v>78</v>
+      <c r="F32" s="10" t="s">
+        <v>41</v>
       </c>
       <c r="N32" s="3" t="s">
         <v>78</v>

</xml_diff>